<commit_message>
Consigue Toda la Informacion Correcta
</commit_message>
<xml_diff>
--- a/player_data.xlsx
+++ b/player_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,10 +441,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Position</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Age</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Nation</t>
         </is>
@@ -458,10 +463,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Second Striker</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>39</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -475,10 +485,15 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Defensive Midfield</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>39</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
@@ -492,10 +507,15 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Central Midfield</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>25</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Uruguay</t>
         </is>
@@ -509,10 +529,15 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Centre-Back</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>45</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -526,10 +551,15 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Central Midfield</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>34</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -543,10 +573,15 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>Defensive Midfield</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>28</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -560,10 +595,15 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>Defence</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>77</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -577,10 +617,15 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>Attacking Midfield</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>35</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -594,10 +639,15 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Right Winger</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>32</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -611,10 +661,15 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>Attacking Midfield</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>44</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -628,10 +683,15 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>Central Midfield</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>24</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -645,10 +705,15 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>Left Winger</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>38</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -662,10 +727,15 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>Centre-Back</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>42</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -679,10 +749,15 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>Defensive Midfield</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>42</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -696,10 +771,15 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>Centre-Back</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>33</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -713,10 +793,15 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>Goalkeeper</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>50</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -730,10 +815,15 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>Central Midfield</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>48</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -747,10 +837,15 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>Centre-Forward</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>50</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -764,10 +859,15 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>Centre-Back</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>61</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -781,10 +881,15 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>Central Midfield</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>90</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>Brazil</t>
         </is>
@@ -798,10 +903,15 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>Attacking Midfield</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>†60</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -815,10 +925,15 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>Centre-Back</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>44</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>Colombia</t>
         </is>
@@ -832,10 +947,15 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>Goalkeeper</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>41</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -849,10 +969,15 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>Central Midfield</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>27</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Uruguay</t>
         </is>
@@ -866,10 +991,15 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>Right-Back</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>49</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -883,10 +1013,15 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>Centre-Forward</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>35</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -900,10 +1035,15 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>Centre-Forward</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
           <t>37</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>Colombia</t>
         </is>
@@ -917,10 +1057,15 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>Centre-Forward</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>34</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>Chile</t>
         </is>
@@ -934,10 +1079,15 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>Centre-Forward</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
           <t>45</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>France</t>
         </is>
@@ -951,10 +1101,15 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
+          <t>Left Winger</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
           <t>28</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -968,10 +1123,15 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>Second Striker</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
           <t>†88</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>Spain</t>
         </is>
@@ -985,10 +1145,15 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t>Defensive Midfield</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
           <t>38</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1002,10 +1167,15 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>Defensive Midfield</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
           <t>42</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1019,10 +1189,15 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>Sweeper</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
           <t>69</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1036,10 +1211,15 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
+          <t>Defence</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
           <t>77</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1053,10 +1233,15 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>Centre-Forward</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
           <t>23</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1070,10 +1255,15 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
+          <t>Defensive Midfield</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
           <t>37</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1087,10 +1277,15 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>Defensive Midfield</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
           <t>22</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1104,10 +1299,15 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>Defensive Midfield</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
           <t>29</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1121,10 +1321,15 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>Attacking Midfield</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
           <t>43</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1138,10 +1343,15 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
+          <t>Second Striker</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
           <t>41</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1155,10 +1365,15 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
+          <t>Central Midfield</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
           <t>42</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1172,10 +1387,15 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>Centre-Forward</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
           <t>27</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>Colombia</t>
         </is>
@@ -1189,10 +1409,15 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>Right Winger</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
           <t>31</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1206,10 +1431,15 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>Centre-Forward</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
           <t>27</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1223,10 +1453,15 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
+          <t>Central Midfield</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
           <t>24</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1240,10 +1475,15 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
+          <t>Attacking Midfield</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
           <t>29</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1257,10 +1497,15 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>Centre-Forward</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
           <t>47</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1274,10 +1519,15 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>Centre-Back</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
           <t>61</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1291,10 +1541,15 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>Goalkeeper</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
           <t>65</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1308,10 +1563,15 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
+          <t>Right Winger</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
           <t>28</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1325,10 +1585,15 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
+          <t>Second Striker</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
           <t>†62</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>Spain</t>
         </is>
@@ -1342,10 +1607,15 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
+          <t>Left Winger</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
           <t>38</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1359,10 +1629,15 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
+          <t>Centre-Back</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
           <t>61</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="D55" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1376,10 +1651,15 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
+          <t>Centre-Back</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
           <t>71</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1393,10 +1673,15 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
+          <t>Centre-Back</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
           <t>46</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>Colombia</t>
         </is>
@@ -1410,10 +1695,15 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
+          <t>Defensive Midfield</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
           <t>†82</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t>Italy</t>
         </is>
@@ -1427,10 +1717,15 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
+          <t>Left Winger</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
           <t>†84</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="D59" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1444,10 +1739,15 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
+          <t>Centre-Back</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
           <t>26</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1461,10 +1761,15 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
+          <t>Left Midfield</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
           <t>46</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1478,10 +1783,15 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
+          <t>Attacking Midfield</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
           <t>75</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="D62" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1495,10 +1805,15 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
+          <t>Goalkeeper</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
           <t>71</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="D63" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1512,10 +1827,15 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
+          <t>Left Winger</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
           <t>70</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="D64" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1529,10 +1849,15 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
+          <t>Right-Back</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
           <t>38</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="D65" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1546,10 +1871,15 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
+          <t>Left Winger</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
           <t>35</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="D66" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1563,10 +1893,15 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
+          <t>Midfield</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
           <t>85</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="D67" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1580,10 +1915,15 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
+          <t>Central Midfield</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
           <t>39</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="D68" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1597,10 +1937,15 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
+          <t>Attacking Midfield</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
           <t>42</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="D69" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1614,10 +1959,15 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
+          <t>Centre-Back</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
           <t>32</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="D70" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1631,10 +1981,15 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
+          <t>Centre-Forward</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
           <t>29</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1648,10 +2003,15 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
+          <t>Attacking Midfield</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
           <t>39</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1665,10 +2025,15 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
+          <t>Midfield</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
           <t>†72</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="D73" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1682,10 +2047,15 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
+          <t>Centre-Back</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
           <t>39</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="D74" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>
@@ -1699,10 +2069,15 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
+          <t>Centre-Back</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
           <t>36</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="D75" t="inlineStr">
         <is>
           <t>Colombia</t>
         </is>
@@ -1716,10 +2091,15 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
+          <t>Defence</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
           <t>†72</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="D76" t="inlineStr">
         <is>
           <t>Argentina</t>
         </is>

</xml_diff>